<commit_message>
R11 CZ data import
</commit_message>
<xml_diff>
--- a/tables/variables.xlsx
+++ b/tables/variables.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t xml:space="preserve">ESS11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS11SC</t>
   </si>
   <si>
     <t xml:space="preserve">flag</t>
@@ -680,8 +683,9 @@
     <col min="6" max="6" width="5.71" hidden="0" customWidth="1"/>
     <col min="7" max="7" width="7.71" hidden="0" customWidth="1"/>
     <col min="8" max="8" width="5.71" hidden="0" customWidth="1"/>
-    <col min="9" max="9" width="4.71" hidden="0" customWidth="1"/>
-    <col min="10" max="10" width="99.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="7.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="4.71" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="99.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -715,13 +719,16 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -742,18 +749,21 @@
         <v>1</v>
       </c>
       <c r="I2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
@@ -774,18 +784,21 @@
         <v>1</v>
       </c>
       <c r="I3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
@@ -806,18 +819,21 @@
         <v>1</v>
       </c>
       <c r="I4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -838,18 +854,21 @@
         <v>1</v>
       </c>
       <c r="I5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
@@ -870,18 +889,21 @@
         <v>1</v>
       </c>
       <c r="I6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" t="b">
         <v>1</v>
@@ -902,18 +924,21 @@
         <v>1</v>
       </c>
       <c r="I7" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>22</v>
+        <v>1</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" t="b">
         <v>1</v>
@@ -934,18 +959,21 @@
         <v>1</v>
       </c>
       <c r="I8" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" t="b">
         <v>1</v>
@@ -966,18 +994,21 @@
         <v>1</v>
       </c>
       <c r="I9" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>26</v>
+        <v>1</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
@@ -998,18 +1029,21 @@
         <v>1</v>
       </c>
       <c r="I10" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" t="s">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -1030,18 +1064,21 @@
         <v>1</v>
       </c>
       <c r="I11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" t="s">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -1062,18 +1099,21 @@
         <v>1</v>
       </c>
       <c r="I12" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" t="b">
         <v>1</v>
@@ -1094,50 +1134,56 @@
         <v>1</v>
       </c>
       <c r="I13" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" t="s">
-        <v>35</v>
+        <v>1</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
         <v>36</v>
-      </c>
-      <c r="C14" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" t="b">
         <v>1</v>
@@ -1158,18 +1204,21 @@
         <v>1</v>
       </c>
       <c r="I15" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" t="b">
         <v>1</v>
@@ -1190,18 +1239,21 @@
         <v>1</v>
       </c>
       <c r="I16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" t="s">
-        <v>35</v>
+        <v>1</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C17" t="b">
         <v>1</v>
@@ -1222,18 +1274,21 @@
         <v>1</v>
       </c>
       <c r="I17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C18" t="b">
         <v>1</v>
@@ -1254,18 +1309,21 @@
         <v>1</v>
       </c>
       <c r="I18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -1286,18 +1344,21 @@
         <v>1</v>
       </c>
       <c r="I19" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -1318,18 +1379,21 @@
         <v>1</v>
       </c>
       <c r="I20" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C21" t="b">
         <v>1</v>
@@ -1350,18 +1414,21 @@
         <v>1</v>
       </c>
       <c r="I21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C22" t="b">
         <v>1</v>
@@ -1382,18 +1449,21 @@
         <v>1</v>
       </c>
       <c r="I22" t="b">
-        <v>0</v>
-      </c>
-      <c r="J22" t="s">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C23" t="b">
         <v>1</v>
@@ -1414,18 +1484,21 @@
         <v>1</v>
       </c>
       <c r="I23" t="b">
-        <v>0</v>
-      </c>
-      <c r="J23" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C24" t="b">
         <v>1</v>
@@ -1446,18 +1519,21 @@
         <v>1</v>
       </c>
       <c r="I24" t="b">
-        <v>0</v>
-      </c>
-      <c r="J24" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C25" t="b">
         <v>1</v>
@@ -1478,18 +1554,21 @@
         <v>1</v>
       </c>
       <c r="I25" t="b">
-        <v>0</v>
-      </c>
-      <c r="J25" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C26" t="b">
         <v>1</v>
@@ -1510,18 +1589,21 @@
         <v>1</v>
       </c>
       <c r="I26" t="b">
-        <v>0</v>
-      </c>
-      <c r="J26" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J26" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C27" t="b">
         <v>1</v>
@@ -1542,18 +1624,21 @@
         <v>1</v>
       </c>
       <c r="I27" t="b">
-        <v>0</v>
-      </c>
-      <c r="J27" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C28" t="b">
         <v>1</v>
@@ -1574,18 +1659,21 @@
         <v>1</v>
       </c>
       <c r="I28" t="b">
-        <v>0</v>
-      </c>
-      <c r="J28" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C29" t="b">
         <v>1</v>
@@ -1606,18 +1694,21 @@
         <v>1</v>
       </c>
       <c r="I29" t="b">
-        <v>0</v>
-      </c>
-      <c r="J29" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J29" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C30" t="b">
         <v>1</v>
@@ -1638,18 +1729,21 @@
         <v>1</v>
       </c>
       <c r="I30" t="b">
-        <v>0</v>
-      </c>
-      <c r="J30" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K30" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C31" t="b">
         <v>1</v>
@@ -1670,18 +1764,21 @@
         <v>1</v>
       </c>
       <c r="I31" t="b">
-        <v>0</v>
-      </c>
-      <c r="J31" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J31" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C32" t="b">
         <v>1</v>
@@ -1702,18 +1799,21 @@
         <v>1</v>
       </c>
       <c r="I32" t="b">
-        <v>0</v>
-      </c>
-      <c r="J32" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C33" t="b">
         <v>1</v>
@@ -1734,18 +1834,21 @@
         <v>1</v>
       </c>
       <c r="I33" t="b">
-        <v>0</v>
-      </c>
-      <c r="J33" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J33" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C34" t="b">
         <v>1</v>
@@ -1766,18 +1869,21 @@
         <v>1</v>
       </c>
       <c r="I34" t="b">
-        <v>0</v>
-      </c>
-      <c r="J34" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C35" t="b">
         <v>1</v>
@@ -1798,18 +1904,21 @@
         <v>1</v>
       </c>
       <c r="I35" t="b">
-        <v>0</v>
-      </c>
-      <c r="J35" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J35" t="b">
+        <v>0</v>
+      </c>
+      <c r="K35" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C36" t="b">
         <v>1</v>
@@ -1830,18 +1939,21 @@
         <v>1</v>
       </c>
       <c r="I36" t="b">
-        <v>0</v>
-      </c>
-      <c r="J36" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J36" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C37" t="b">
         <v>1</v>
@@ -1862,18 +1974,21 @@
         <v>1</v>
       </c>
       <c r="I37" t="b">
-        <v>0</v>
-      </c>
-      <c r="J37" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J37" t="b">
+        <v>0</v>
+      </c>
+      <c r="K37" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C38" t="b">
         <v>1</v>
@@ -1894,18 +2009,21 @@
         <v>1</v>
       </c>
       <c r="I38" t="b">
-        <v>0</v>
-      </c>
-      <c r="J38" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J38" t="b">
+        <v>0</v>
+      </c>
+      <c r="K38" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C39" t="b">
         <v>1</v>
@@ -1926,18 +2044,21 @@
         <v>1</v>
       </c>
       <c r="I39" t="b">
-        <v>0</v>
-      </c>
-      <c r="J39" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J39" t="b">
+        <v>0</v>
+      </c>
+      <c r="K39" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B40" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C40" t="b">
         <v>1</v>
@@ -1958,18 +2079,21 @@
         <v>1</v>
       </c>
       <c r="I40" t="b">
-        <v>0</v>
-      </c>
-      <c r="J40" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="J40" t="b">
+        <v>0</v>
+      </c>
+      <c r="K40" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B41" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C41" t="b">
         <v>1</v>
@@ -1990,50 +2114,56 @@
         <v>1</v>
       </c>
       <c r="I41" t="b">
-        <v>0</v>
-      </c>
-      <c r="J41" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="J41" t="b">
+        <v>0</v>
+      </c>
+      <c r="K41" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" t="b">
+        <v>1</v>
+      </c>
+      <c r="E42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
+      <c r="J42" t="b">
+        <v>0</v>
+      </c>
+      <c r="K42" t="s">
         <v>66</v>
-      </c>
-      <c r="C42" t="b">
-        <v>1</v>
-      </c>
-      <c r="D42" t="b">
-        <v>1</v>
-      </c>
-      <c r="E42" t="b">
-        <v>1</v>
-      </c>
-      <c r="F42" t="b">
-        <v>1</v>
-      </c>
-      <c r="G42" t="b">
-        <v>1</v>
-      </c>
-      <c r="H42" t="b">
-        <v>1</v>
-      </c>
-      <c r="I42" t="b">
-        <v>0</v>
-      </c>
-      <c r="J42" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C43" t="b">
         <v>1</v>
@@ -2054,18 +2184,21 @@
         <v>1</v>
       </c>
       <c r="I43" t="b">
-        <v>0</v>
-      </c>
-      <c r="J43" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="J43" t="b">
+        <v>0</v>
+      </c>
+      <c r="K43" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B44" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C44" t="b">
         <v>1</v>
@@ -2086,18 +2219,21 @@
         <v>1</v>
       </c>
       <c r="I44" t="b">
-        <v>0</v>
-      </c>
-      <c r="J44" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="J44" t="b">
+        <v>0</v>
+      </c>
+      <c r="K44" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B45" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C45" t="b">
         <v>1</v>
@@ -2118,18 +2254,21 @@
         <v>1</v>
       </c>
       <c r="I45" t="b">
-        <v>0</v>
-      </c>
-      <c r="J45" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="J45" t="b">
+        <v>0</v>
+      </c>
+      <c r="K45" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B46" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C46" t="b">
         <v>1</v>
@@ -2150,18 +2289,21 @@
         <v>1</v>
       </c>
       <c r="I46" t="b">
-        <v>0</v>
-      </c>
-      <c r="J46" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="J46" t="b">
+        <v>0</v>
+      </c>
+      <c r="K46" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B47" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C47" t="b">
         <v>1</v>
@@ -2182,18 +2324,21 @@
         <v>1</v>
       </c>
       <c r="I47" t="b">
-        <v>0</v>
-      </c>
-      <c r="J47" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="J47" t="b">
+        <v>0</v>
+      </c>
+      <c r="K47" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B48" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C48" t="b">
         <v>1</v>
@@ -2214,50 +2359,56 @@
         <v>1</v>
       </c>
       <c r="I48" t="b">
-        <v>0</v>
-      </c>
-      <c r="J48" t="s">
-        <v>73</v>
+        <v>1</v>
+      </c>
+      <c r="J48" t="b">
+        <v>0</v>
+      </c>
+      <c r="K48" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B49" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" t="b">
+        <v>1</v>
+      </c>
+      <c r="D49" t="b">
+        <v>1</v>
+      </c>
+      <c r="E49" t="b">
+        <v>1</v>
+      </c>
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
+      <c r="G49" t="b">
+        <v>0</v>
+      </c>
+      <c r="H49" t="b">
+        <v>1</v>
+      </c>
+      <c r="I49" t="b">
+        <v>0</v>
+      </c>
+      <c r="J49" t="b">
+        <v>1</v>
+      </c>
+      <c r="K49" t="s">
         <v>74</v>
-      </c>
-      <c r="C49" t="b">
-        <v>1</v>
-      </c>
-      <c r="D49" t="b">
-        <v>1</v>
-      </c>
-      <c r="E49" t="b">
-        <v>1</v>
-      </c>
-      <c r="F49" t="b">
-        <v>1</v>
-      </c>
-      <c r="G49" t="b">
-        <v>0</v>
-      </c>
-      <c r="H49" t="b">
-        <v>1</v>
-      </c>
-      <c r="I49" t="b">
-        <v>1</v>
-      </c>
-      <c r="J49" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B50" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C50" t="b">
         <v>1</v>
@@ -2278,18 +2429,21 @@
         <v>1</v>
       </c>
       <c r="I50" t="b">
-        <v>0</v>
-      </c>
-      <c r="J50" t="s">
-        <v>73</v>
+        <v>1</v>
+      </c>
+      <c r="J50" t="b">
+        <v>0</v>
+      </c>
+      <c r="K50" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B51" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C51" t="b">
         <v>1</v>
@@ -2310,18 +2464,21 @@
         <v>1</v>
       </c>
       <c r="I51" t="b">
-        <v>0</v>
-      </c>
-      <c r="J51" t="s">
-        <v>73</v>
+        <v>1</v>
+      </c>
+      <c r="J51" t="b">
+        <v>0</v>
+      </c>
+      <c r="K51" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C52" t="b">
         <v>1</v>
@@ -2342,18 +2499,21 @@
         <v>1</v>
       </c>
       <c r="I52" t="b">
-        <v>0</v>
-      </c>
-      <c r="J52" t="s">
-        <v>73</v>
+        <v>1</v>
+      </c>
+      <c r="J52" t="b">
+        <v>0</v>
+      </c>
+      <c r="K52" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C53" t="b">
         <v>1</v>
@@ -2374,18 +2534,21 @@
         <v>1</v>
       </c>
       <c r="I53" t="b">
-        <v>0</v>
-      </c>
-      <c r="J53" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="J53" t="b">
+        <v>0</v>
+      </c>
+      <c r="K53" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C54" t="b">
         <v>1</v>
@@ -2406,18 +2569,21 @@
         <v>1</v>
       </c>
       <c r="I54" t="b">
-        <v>0</v>
-      </c>
-      <c r="J54" t="s">
-        <v>73</v>
+        <v>1</v>
+      </c>
+      <c r="J54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K54" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C55" t="b">
         <v>1</v>
@@ -2438,18 +2604,21 @@
         <v>1</v>
       </c>
       <c r="I55" t="b">
-        <v>0</v>
-      </c>
-      <c r="J55" t="s">
-        <v>73</v>
+        <v>1</v>
+      </c>
+      <c r="J55" t="b">
+        <v>0</v>
+      </c>
+      <c r="K55" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C56" t="b">
         <v>1</v>
@@ -2470,18 +2639,21 @@
         <v>1</v>
       </c>
       <c r="I56" t="b">
-        <v>0</v>
-      </c>
-      <c r="J56" t="s">
-        <v>73</v>
+        <v>1</v>
+      </c>
+      <c r="J56" t="b">
+        <v>0</v>
+      </c>
+      <c r="K56" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B57" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C57" t="b">
         <v>1</v>
@@ -2502,18 +2674,21 @@
         <v>1</v>
       </c>
       <c r="I57" t="b">
-        <v>0</v>
-      </c>
-      <c r="J57" t="s">
-        <v>73</v>
+        <v>1</v>
+      </c>
+      <c r="J57" t="b">
+        <v>0</v>
+      </c>
+      <c r="K57" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C58" t="b">
         <v>1</v>
@@ -2534,18 +2709,21 @@
         <v>1</v>
       </c>
       <c r="I58" t="b">
-        <v>0</v>
-      </c>
-      <c r="J58" t="s">
-        <v>73</v>
+        <v>1</v>
+      </c>
+      <c r="J58" t="b">
+        <v>0</v>
+      </c>
+      <c r="K58" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B59" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C59" t="b">
         <v>1</v>
@@ -2566,18 +2744,21 @@
         <v>1</v>
       </c>
       <c r="I59" t="b">
-        <v>0</v>
-      </c>
-      <c r="J59" t="s">
-        <v>73</v>
+        <v>1</v>
+      </c>
+      <c r="J59" t="b">
+        <v>0</v>
+      </c>
+      <c r="K59" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C60" t="b">
         <v>1</v>
@@ -2598,18 +2779,21 @@
         <v>1</v>
       </c>
       <c r="I60" t="b">
-        <v>1</v>
-      </c>
-      <c r="J60" t="s">
-        <v>73</v>
+        <v>0</v>
+      </c>
+      <c r="J60" t="b">
+        <v>1</v>
+      </c>
+      <c r="K60" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C61" t="b">
         <v>1</v>
@@ -2630,18 +2814,21 @@
         <v>1</v>
       </c>
       <c r="I61" t="b">
-        <v>0</v>
-      </c>
-      <c r="J61" t="s">
-        <v>73</v>
+        <v>1</v>
+      </c>
+      <c r="J61" t="b">
+        <v>0</v>
+      </c>
+      <c r="K61" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C62" t="b">
         <v>1</v>
@@ -2662,18 +2849,21 @@
         <v>1</v>
       </c>
       <c r="I62" t="b">
-        <v>0</v>
-      </c>
-      <c r="J62" t="s">
-        <v>73</v>
+        <v>1</v>
+      </c>
+      <c r="J62" t="b">
+        <v>0</v>
+      </c>
+      <c r="K62" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
@@ -2694,16 +2884,19 @@
         <v>0</v>
       </c>
       <c r="I63" t="b">
-        <v>1</v>
-      </c>
-      <c r="J63"/>
+        <v>0</v>
+      </c>
+      <c r="J63" t="b">
+        <v>1</v>
+      </c>
+      <c r="K63"/>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C64" t="b">
         <v>1</v>
@@ -2724,18 +2917,21 @@
         <v>1</v>
       </c>
       <c r="I64" t="b">
-        <v>0</v>
-      </c>
-      <c r="J64" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="J64" t="b">
+        <v>0</v>
+      </c>
+      <c r="K64" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C65" t="b">
         <v>1</v>
@@ -2756,18 +2952,21 @@
         <v>1</v>
       </c>
       <c r="I65" t="b">
-        <v>0</v>
-      </c>
-      <c r="J65" t="s">
-        <v>91</v>
+        <v>1</v>
+      </c>
+      <c r="J65" t="b">
+        <v>0</v>
+      </c>
+      <c r="K65" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C66" t="b">
         <v>1</v>
@@ -2788,18 +2987,21 @@
         <v>1</v>
       </c>
       <c r="I66" t="b">
-        <v>0</v>
-      </c>
-      <c r="J66" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="J66" t="b">
+        <v>0</v>
+      </c>
+      <c r="K66" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B67" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C67" t="b">
         <v>1</v>
@@ -2820,18 +3022,21 @@
         <v>1</v>
       </c>
       <c r="I67" t="b">
-        <v>0</v>
-      </c>
-      <c r="J67" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="J67" t="b">
+        <v>0</v>
+      </c>
+      <c r="K67" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B68" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C68" t="b">
         <v>0</v>
@@ -2852,16 +3057,19 @@
         <v>0</v>
       </c>
       <c r="I68" t="b">
-        <v>1</v>
-      </c>
-      <c r="J68"/>
+        <v>0</v>
+      </c>
+      <c r="J68" t="b">
+        <v>1</v>
+      </c>
+      <c r="K68"/>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B69" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C69" t="b">
         <v>1</v>
@@ -2882,18 +3090,21 @@
         <v>1</v>
       </c>
       <c r="I69" t="b">
-        <v>0</v>
-      </c>
-      <c r="J69" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="J69" t="b">
+        <v>0</v>
+      </c>
+      <c r="K69" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B70" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C70" t="b">
         <v>1</v>
@@ -2914,18 +3125,21 @@
         <v>1</v>
       </c>
       <c r="I70" t="b">
-        <v>0</v>
-      </c>
-      <c r="J70" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="J70" t="b">
+        <v>0</v>
+      </c>
+      <c r="K70" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B71" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C71" t="b">
         <v>1</v>
@@ -2946,18 +3160,21 @@
         <v>1</v>
       </c>
       <c r="I71" t="b">
-        <v>0</v>
-      </c>
-      <c r="J71" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="J71" t="b">
+        <v>0</v>
+      </c>
+      <c r="K71" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B72" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C72" t="b">
         <v>1</v>
@@ -2978,18 +3195,21 @@
         <v>1</v>
       </c>
       <c r="I72" t="b">
-        <v>1</v>
-      </c>
-      <c r="J72" t="s">
-        <v>65</v>
+        <v>0</v>
+      </c>
+      <c r="J72" t="b">
+        <v>1</v>
+      </c>
+      <c r="K72" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B73" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C73" t="b">
         <v>1</v>
@@ -3010,18 +3230,21 @@
         <v>1</v>
       </c>
       <c r="I73" t="b">
-        <v>1</v>
-      </c>
-      <c r="J73" t="s">
-        <v>65</v>
+        <v>0</v>
+      </c>
+      <c r="J73" t="b">
+        <v>1</v>
+      </c>
+      <c r="K73" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B74" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C74" t="b">
         <v>0</v>
@@ -3044,16 +3267,19 @@
       <c r="I74" t="b">
         <v>1</v>
       </c>
-      <c r="J74" t="s">
-        <v>91</v>
+      <c r="J74" t="b">
+        <v>1</v>
+      </c>
+      <c r="K74" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B75" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C75" t="b">
         <v>1</v>
@@ -3074,18 +3300,21 @@
         <v>1</v>
       </c>
       <c r="I75" t="b">
-        <v>0</v>
-      </c>
-      <c r="J75" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="J75" t="b">
+        <v>0</v>
+      </c>
+      <c r="K75" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B76" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C76" t="b">
         <v>1</v>
@@ -3106,18 +3335,21 @@
         <v>1</v>
       </c>
       <c r="I76" t="b">
-        <v>0</v>
-      </c>
-      <c r="J76" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="J76" t="b">
+        <v>0</v>
+      </c>
+      <c r="K76" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B77" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C77" t="b">
         <v>1</v>
@@ -3138,18 +3370,21 @@
         <v>1</v>
       </c>
       <c r="I77" t="b">
-        <v>0</v>
-      </c>
-      <c r="J77" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="J77" t="b">
+        <v>0</v>
+      </c>
+      <c r="K77" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B78" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C78" t="b">
         <v>1</v>
@@ -3170,18 +3405,21 @@
         <v>1</v>
       </c>
       <c r="I78" t="b">
-        <v>0</v>
-      </c>
-      <c r="J78" t="s">
-        <v>91</v>
+        <v>1</v>
+      </c>
+      <c r="J78" t="b">
+        <v>0</v>
+      </c>
+      <c r="K78" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B79" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C79" t="b">
         <v>1</v>
@@ -3202,10 +3440,13 @@
         <v>1</v>
       </c>
       <c r="I79" t="b">
-        <v>0</v>
-      </c>
-      <c r="J79" t="s">
-        <v>65</v>
+        <v>1</v>
+      </c>
+      <c r="J79" t="b">
+        <v>0</v>
+      </c>
+      <c r="K79" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>